<commit_message>
feat: vocabularies and grammar
</commit_message>
<xml_diff>
--- a/English/Vocabularies.xlsx
+++ b/English/Vocabularies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubRepository\LearningNotes\English\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD83DF1-3F0F-40A7-8441-908B530D476C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662994DA-B3F1-4240-AEA5-853C8E40AE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="624" windowWidth="10692" windowHeight="11976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12192" yWindow="264" windowWidth="10692" windowHeight="11976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="2326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="2508">
   <si>
     <t>port</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -23684,6 +23684,2088 @@
   </si>
   <si>
     <t>便宜的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>trim</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>调整</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>修剪</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>减少</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>recession</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>衰退</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  odd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>几率</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>recede</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>减弱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>proceed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>进行</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>further</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>进一步</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>monetary</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tighten</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>收紧</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>affirm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>声明</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>肯定</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>steady</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>稳重, 稳定, 稳住</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>直接的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>直的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>captive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>被俘的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kidnap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>绑架</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>contention</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rescind</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loyalist</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>忠诚者</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ballot</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>投票否决</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>paralysis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>瘫痪</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nomination</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>提名</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>representative</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>n.代表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>advisory</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>顾问的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>over-the-counter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>非处方的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>determined</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>确定</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pension</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>退休金, 抚恤金, 津贴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pensioner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>领养老金</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>抚恤金者</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dispense</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分配</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分发</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dispensation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>indispensable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>indispensability</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不可或缺的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>必要的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>同</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>necessary)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>compensate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>补偿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>赔偿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>抵消</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>compensation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>compensatory</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uncompensated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overcompensate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overcompensatation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>well-compensated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得充分赔偿的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>perpend</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>深思</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>慎重考虑</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>仔细考虑</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ponder</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>仔细考虑</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>衡量</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>沉思</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ponderable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可衡量的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可估量的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>imponderable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无法计算的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无重量的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>preponderabce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>优势</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>占优势</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>preponderant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>突出的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>压倒性的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ponderous</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>沉重的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>笨重的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>呆板的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ponderously</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>笨重地</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>单板地</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>similar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>sim|sem|simil|sembl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>像</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>similarly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>similarity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>仿性</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>similitude</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>类似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>类似物</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissimilar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不同的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不一样的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissimilarity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissimilate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使变得不同</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissimilation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>disimilitude</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>disimulate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>演示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>假装</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>装糊涂</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>disimulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simulate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模仿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>像</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>假装</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simulator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simulated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>computer-simulated</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机模拟的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模拟的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>仿造的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assimulate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>吸收</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>同化</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>消化</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assimilation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>吸收</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>消化</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assimilator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assimilatative</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simultaneous</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>同时发生的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>同时存在的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simultaneously</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simultaneity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>verisimilar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>似乎是真的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>貌似真实的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>verisimilitude</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>resemble</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相似</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>resumblance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>类似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相似</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相似之处</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>resemblant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>相似的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assemble</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>集合</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>聚集</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>装配</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>收集</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assembly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assembled</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assembler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>汇编程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>汇编机</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>装配工</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assembling</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>装配</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>组合的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reassemble</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>重新装配, 重新召集</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reassimbly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assembly line</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>流水线</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissemble</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">拆开, 废除 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissembled</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissembly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>subassembly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>组价</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>部件</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>unassembled</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>未装配的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pre-assembled</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>预装配的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>self-assembly</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自行组装的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>simile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>明喻</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symphony</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交响乐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交响曲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交响乐团</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symphonic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交响乐的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和声的</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>共生</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合作关系</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>共栖</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symbiosis</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symbiotic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>共生的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symbiotically</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symbiote</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>共生生物</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symbiont</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>共生者</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>synonym</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同义词</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symptom</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>症状</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symptomless</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无症状的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symptomatic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>有症状的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>asymptomatic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symptomatically</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symptom-free</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无症状</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symmetry</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对称</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>整齐</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>asymmetry</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不对称</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symmetrical</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>asymmetrical</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>symmetrically</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>asymmetrically</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -24143,10 +26225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1199"/>
+  <dimension ref="A1:F1283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1176" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1200" sqref="D1200"/>
+    <sheetView tabSelected="1" topLeftCell="C1266" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1284" sqref="C1284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -27058,28 +29140,55 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>7</v>
+        <v>2326</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>2327</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>2328</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>2329</v>
+      </c>
       <c r="C242" s="2" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>2331</v>
+      </c>
       <c r="C243" s="2" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>2333</v>
+      </c>
       <c r="C244" s="2" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>2335</v>
+      </c>
       <c r="C245" s="2" t="s">
         <v>320</v>
       </c>
@@ -27088,11 +29197,23 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>2337</v>
+      </c>
       <c r="C246" s="2" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="C247" s="2" t="s">
         <v>323</v>
       </c>
@@ -27101,6 +29222,12 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>2339</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>2340</v>
+      </c>
       <c r="C248" s="2" t="s">
         <v>324</v>
       </c>
@@ -27109,6 +29236,12 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>2341</v>
+      </c>
+      <c r="B249" s="8" t="s">
+        <v>2342</v>
+      </c>
       <c r="C249" s="2" t="s">
         <v>327</v>
       </c>
@@ -27117,26 +29250,56 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>2343</v>
+      </c>
+      <c r="B250" s="9" t="s">
+        <v>2344</v>
+      </c>
       <c r="C250" s="2" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B251" s="8" t="s">
+        <v>2345</v>
+      </c>
       <c r="C251" s="2" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>2347</v>
+      </c>
       <c r="C252" s="2" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>2348</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>2349</v>
+      </c>
       <c r="C253" s="2" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>2350</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>401</v>
+      </c>
       <c r="C254" s="2" t="s">
         <v>333</v>
       </c>
@@ -27145,6 +29308,12 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>2352</v>
+      </c>
       <c r="C255" s="2" t="s">
         <v>335</v>
       </c>
@@ -27153,31 +29322,67 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>2354</v>
+      </c>
       <c r="C256" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="257" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>2356</v>
+      </c>
       <c r="C257" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="258" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>2357</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>2358</v>
+      </c>
       <c r="C258" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="259" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>2360</v>
+      </c>
       <c r="C259" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="260" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>2361</v>
+      </c>
+      <c r="B260" s="9" t="s">
+        <v>2362</v>
+      </c>
       <c r="C260" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="261" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>2364</v>
+      </c>
       <c r="C261" s="2" t="s">
         <v>342</v>
       </c>
@@ -27185,37 +29390,49 @@
         <v>343</v>
       </c>
     </row>
-    <row r="262" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>2365</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>2366</v>
+      </c>
       <c r="C262" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="263" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>2368</v>
+      </c>
       <c r="C263" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="264" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C264" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="265" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C265" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="266" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C266" s="2" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="267" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C267" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="268" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C268" s="2" t="s">
         <v>350</v>
       </c>
@@ -27223,12 +29440,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="269" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C269" s="2" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="270" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C270" s="2" t="s">
         <v>353</v>
       </c>
@@ -27236,7 +29453,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="271" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C271" s="2" t="s">
         <v>355</v>
       </c>
@@ -27244,7 +29461,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="272" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C272" s="2" t="s">
         <v>356</v>
       </c>
@@ -33620,8 +35837,597 @@
       </c>
     </row>
     <row r="1199" spans="3:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C1199" s="7"/>
-      <c r="D1199" s="5"/>
+      <c r="C1199" s="7" t="s">
+        <v>2369</v>
+      </c>
+      <c r="D1199" s="5" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="1200" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1200" s="2" t="s">
+        <v>2371</v>
+      </c>
+      <c r="D1200" s="4" t="s">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="1201" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1201" s="2" t="s">
+        <v>2373</v>
+      </c>
+      <c r="D1201" s="4" t="s">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="1202" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1202" s="2" t="s">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="1203" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1203" s="2" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D1203" s="4" t="s">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="1204" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1204" s="2" t="s">
+        <v>2377</v>
+      </c>
+    </row>
+    <row r="1205" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1205" s="2" t="s">
+        <v>2379</v>
+      </c>
+      <c r="D1205" s="4" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="1206" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1206" s="2" t="s">
+        <v>2381</v>
+      </c>
+    </row>
+    <row r="1207" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1207" s="2" t="s">
+        <v>2382</v>
+      </c>
+      <c r="D1207" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1208" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1208" s="2" t="s">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="1209" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1209" s="2" t="s">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="1210" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1210" s="2" t="s">
+        <v>2385</v>
+      </c>
+    </row>
+    <row r="1211" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1211" s="2" t="s">
+        <v>2386</v>
+      </c>
+      <c r="D1211" s="5" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="1212" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1212" s="2" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D1212" s="4" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="1213" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1213" s="2" t="s">
+        <v>2390</v>
+      </c>
+      <c r="D1213" s="4" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="1214" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1214" s="2" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D1214" s="4" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="1215" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1215" s="2" t="s">
+        <v>2394</v>
+      </c>
+      <c r="D1215" s="4" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="1216" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1216" s="2" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D1216" s="4" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="1217" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1217" s="2" t="s">
+        <v>2398</v>
+      </c>
+      <c r="D1217" s="4" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="1218" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1218" s="2" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1218" s="4" t="s">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="1219" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1219" s="2" t="s">
+        <v>2402</v>
+      </c>
+      <c r="D1219" s="4" t="s">
+        <v>2403</v>
+      </c>
+    </row>
+    <row r="1220" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1220" s="2" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D1220" s="1" t="s">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="1221" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1221" s="2" t="s">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="1222" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1222" s="2" t="s">
+        <v>2407</v>
+      </c>
+      <c r="D1222" s="4" t="s">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="1223" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1223" s="2" t="s">
+        <v>2409</v>
+      </c>
+      <c r="D1223" s="4" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="1224" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1224" s="2" t="s">
+        <v>2411</v>
+      </c>
+      <c r="D1224" s="4" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="1225" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1225" s="2" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="1226" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1226" s="2" t="s">
+        <v>2414</v>
+      </c>
+      <c r="D1226" s="5" t="s">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="1227" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1227" s="2" t="s">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="1228" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1228" s="2" t="s">
+        <v>2417</v>
+      </c>
+    </row>
+    <row r="1229" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1229" s="2" t="s">
+        <v>2418</v>
+      </c>
+      <c r="D1229" s="4" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="1230" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1230" s="2" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="1231" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1231" s="2" t="s">
+        <v>2421</v>
+      </c>
+      <c r="D1231" s="4" t="s">
+        <v>2422</v>
+      </c>
+    </row>
+    <row r="1232" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1232" s="2" t="s">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="1233" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1233" s="2" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="1234" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1234" s="2" t="s">
+        <v>2425</v>
+      </c>
+      <c r="D1234" s="4" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="1235" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1235" s="2" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D1235" s="5" t="s">
+        <v>2427</v>
+      </c>
+    </row>
+    <row r="1236" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1236" s="2" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D1236" s="4" t="s">
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="1237" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1237" s="2" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D1237" s="4" t="s">
+        <v>2432</v>
+      </c>
+    </row>
+    <row r="1238" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1238" s="2" t="s">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="1239" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1239" s="2" t="s">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="1240" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1240" s="2" t="s">
+        <v>2435</v>
+      </c>
+      <c r="D1240" s="4" t="s">
+        <v>2436</v>
+      </c>
+    </row>
+    <row r="1241" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1241" s="2" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="1242" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1242" s="2" t="s">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="1243" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1243" s="2" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D1243" s="4" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="1244" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1244" s="2" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="1245" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1245" s="2" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D1245" s="4" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="1246" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1246" s="2" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D1246" s="4" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="1247" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1247" s="2" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D1247" s="5" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="1248" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1248" s="2" t="s">
+        <v>2448</v>
+      </c>
+      <c r="D1248" s="4" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="1249" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1249" s="2" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="1250" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1250" s="2" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="1251" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1251" s="2" t="s">
+        <v>2452</v>
+      </c>
+      <c r="D1251" s="4" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="1252" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1252" s="2" t="s">
+        <v>2454</v>
+      </c>
+      <c r="D1252" s="4" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="1253" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1253" s="2" t="s">
+        <v>2456</v>
+      </c>
+      <c r="D1253" s="5" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="1254" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1254" s="2" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="1255" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1255" s="2" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D1255" s="5" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="1256" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1256" s="2" t="s">
+        <v>2461</v>
+      </c>
+      <c r="D1256" s="5" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="1257" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1257" s="2" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="1258" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1258" s="2" t="s">
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="1259" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1259" s="2" t="s">
+        <v>2465</v>
+      </c>
+      <c r="D1259" s="4" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="1260" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1260" s="2" t="s">
+        <v>2467</v>
+      </c>
+      <c r="D1260" s="5" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="1261" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1261" s="2" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D1261" s="5" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="1262" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1262" s="2" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D1262" s="5" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="1263" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1263" s="2" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D1263" s="5" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="1264" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1264" s="2" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D1264" s="4" t="s">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="1265" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1265" s="2" t="s">
+        <v>2477</v>
+      </c>
+      <c r="D1265" s="4" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="1266" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1266" s="2" t="s">
+        <v>2480</v>
+      </c>
+      <c r="D1266" s="4" t="s">
+        <v>2479</v>
+      </c>
+    </row>
+    <row r="1267" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1267" s="2" t="s">
+        <v>2481</v>
+      </c>
+      <c r="D1267" s="5" t="s">
+        <v>2482</v>
+      </c>
+    </row>
+    <row r="1268" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1268" s="2" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="1269" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1269" s="2" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D1269" s="5" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="1270" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1270" s="2" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D1270" s="5" t="s">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="1271" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1271" s="2" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D1271" s="5" t="s">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="1272" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1272" s="2" t="s">
+        <v>2490</v>
+      </c>
+      <c r="D1272" s="5" t="s">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="1273" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1273" s="2" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D1273" s="5" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="1274" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1274" s="2" t="s">
+        <v>2494</v>
+      </c>
+      <c r="D1274" s="5" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="1275" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1275" s="2" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D1275" s="5" t="s">
+        <v>2493</v>
+      </c>
+    </row>
+    <row r="1276" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1276" s="2" t="s">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="1277" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1277" s="2" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D1277" s="5" t="s">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="1278" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1278" s="2" t="s">
+        <v>2500</v>
+      </c>
+      <c r="D1278" s="4" t="s">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="1279" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1279" s="2" t="s">
+        <v>2502</v>
+      </c>
+      <c r="D1279" s="5" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="1280" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1280" s="2" t="s">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="1281" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1281" s="2" t="s">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="1282" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1282" s="2" t="s">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="1283" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1283" s="2" t="s">
+        <v>2507</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>